<commit_message>
listo para 9 73
</commit_message>
<xml_diff>
--- a/Notas A2.xlsx
+++ b/Notas A2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Insatalar angular2                           </t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>d (directive)</t>
+  </si>
+  <si>
+    <t>Creamos un nuevo servicio</t>
+  </si>
+  <si>
+    <t>ng g s {nombre_servicio}</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G36"/>
+  <dimension ref="B2:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -633,7 +639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:7">
       <c r="B33" t="s">
         <v>24</v>
       </c>
@@ -641,9 +647,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
-      <c r="B36">
-        <v>44</v>
+    <row r="35" spans="2:7" s="2" customFormat="1">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10 157 para empezar http
</commit_message>
<xml_diff>
--- a/Notas A2.xlsx
+++ b/Notas A2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Insatalar angular2                           </t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>ng g s {nombre_servicio}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    --spec false</t>
+  </si>
+  <si>
+    <t>No specs</t>
+  </si>
+  <si>
+    <t>Creamos un nuevo PIPE</t>
+  </si>
+  <si>
+    <t>ng g p {nombre_pipe}</t>
   </si>
 </sst>
 </file>
@@ -452,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G39"/>
+  <dimension ref="B2:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -610,58 +622,83 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:7" s="2" customFormat="1">
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="1" t="s">
+    <row r="23" spans="2:7">
+      <c r="C23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="2" customFormat="1">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
-      <c r="B27" t="s">
+    <row r="28" spans="2:7">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:7" s="2" customFormat="1">
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="1" t="s">
+    <row r="30" spans="2:7" s="2" customFormat="1">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
-      <c r="B33" t="s">
+    <row r="34" spans="2:7">
+      <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:7" s="2" customFormat="1">
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="1" t="s">
+    <row r="36" spans="2:7" s="2" customFormat="1">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
-      <c r="B39" t="s">
+    <row r="40" spans="2:7">
+      <c r="B40" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" s="2" customFormat="1">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>